<commit_message>
feat: update index page layout with new buttons and functionality, add download template feature, and enhance toast notifications
</commit_message>
<xml_diff>
--- a/Plantilla VIsitas Socoval.xlsx
+++ b/Plantilla VIsitas Socoval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\za51560\Documents\Programacion\Acceso Diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D15EA65-7B07-458E-811A-5A701EC2F678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF914FF9-E1C8-4690-AAFB-ABE736B6A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15105" yWindow="-16365" windowWidth="29040" windowHeight="15720" xr2:uid="{019328E3-E67A-48E0-8BD1-339FFC7A2A37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{019328E3-E67A-48E0-8BD1-339FFC7A2A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -392,15 +392,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -422,6 +413,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,7 +759,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,51 +775,51 @@
   <sheetData>
     <row r="1" spans="2:10" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="2:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -828,24 +828,24 @@
       <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="21">
-        <v>46009</v>
+      <c r="I4" s="18">
+        <v>46010</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -854,24 +854,24 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="21">
-        <v>46009</v>
+      <c r="I5" s="18">
+        <v>46010</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -880,28 +880,28 @@
       <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="6">
-        <v>46009</v>
+        <v>46010</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="4"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="24"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4"/>
@@ -911,7 +911,7 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="24"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
@@ -921,7 +921,7 @@
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
@@ -932,7 +932,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
@@ -942,7 +942,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
@@ -952,7 +952,7 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="25"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="7"/>
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>

</xml_diff>